<commit_message>
"#1 started implementing Flask html formatting to supercede both contexts.xlsx manual inputs and conf.py html snippets."
</commit_message>
<xml_diff>
--- a/contexts.xlsx
+++ b/contexts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10910"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aug05\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katrinawheelan/Desktop/Code/CLOSUP/process_xbrl/process-xbrl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2106EA49-A5E9-42E4-904A-071DC7F1034B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0950D10-B10B-2A46-90D7-9696C4EA98D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -742,7 +742,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1106,20 +1106,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D30" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="141" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" customWidth="1"/>
     <col min="2" max="2" width="62" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" customWidth="1"/>
-    <col min="4" max="4" width="59.85546875" customWidth="1"/>
-    <col min="5" max="5" width="145.85546875" customWidth="1"/>
+    <col min="3" max="3" width="29.5" customWidth="1"/>
+    <col min="4" max="4" width="59.83203125" customWidth="1"/>
+    <col min="5" max="5" width="145.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="165">
+    <row r="2" spans="1:5" ht="176" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1146,14 +1146,14 @@
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="165">
+    <row r="3" spans="1:5" ht="176" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1170,7 +1170,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="123" customHeight="1">
+    <row r="4" spans="1:5" ht="123" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1187,7 +1187,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="165">
+    <row r="5" spans="1:5" ht="176" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1204,7 +1204,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="195">
+    <row r="6" spans="1:5" ht="208" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="195">
+    <row r="7" spans="1:5" ht="208" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1238,7 +1238,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="195">
+    <row r="8" spans="1:5" ht="208" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="195">
+    <row r="9" spans="1:5" ht="208" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="195">
+    <row r="10" spans="1:5" ht="208" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1289,7 +1289,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="165">
+    <row r="11" spans="1:5" ht="176" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="180">
+    <row r="12" spans="1:5" ht="192" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="210">
+    <row r="13" spans="1:5" ht="224" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="210">
+    <row r="14" spans="1:5" ht="224" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="210">
+    <row r="15" spans="1:5" ht="224" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="210">
+    <row r="16" spans="1:5" ht="224" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1391,7 +1391,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="210">
+    <row r="17" spans="1:5" ht="224" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="180">
+    <row r="18" spans="1:5" ht="192" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="195">
+    <row r="19" spans="1:5" ht="208" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="195">
+    <row r="20" spans="1:5" ht="208" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="210">
+    <row r="21" spans="1:5" ht="224" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>53</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="210">
+    <row r="22" spans="1:5" ht="224" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="210">
+    <row r="23" spans="1:5" ht="224" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="210">
+    <row r="24" spans="1:5" ht="224" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>53</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="180">
+    <row r="25" spans="1:5" ht="192" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="180">
+    <row r="26" spans="1:5" ht="192" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -1561,7 +1561,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="135">
+    <row r="27" spans="1:5" ht="144" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -1578,7 +1578,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="210">
+    <row r="28" spans="1:5" ht="208" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -1592,7 +1592,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="210">
+    <row r="29" spans="1:5" ht="208" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="210">
+    <row r="30" spans="1:5" ht="208" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="210">
+    <row r="31" spans="1:5" ht="224" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -1634,7 +1634,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="240">
+    <row r="32" spans="1:5" ht="240" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="240">
+    <row r="33" spans="1:5" ht="240" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -1662,7 +1662,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="240">
+    <row r="34" spans="1:5" ht="240" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="210">
+    <row r="35" spans="1:5" ht="208" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="210">
+    <row r="36" spans="1:5" ht="208" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -1704,7 +1704,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="210">
+    <row r="37" spans="1:5" ht="208" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>5</v>
       </c>
@@ -1718,7 +1718,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="180">
+    <row r="38" spans="1:5" ht="192" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="180">
+    <row r="39" spans="1:5" ht="192" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>5</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="180">
+    <row r="40" spans="1:5" ht="192" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>5</v>
       </c>
@@ -1773,72 +1773,72 @@
       <selection sqref="A1:A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="52.85546875" customWidth="1"/>
+    <col min="1" max="1" width="52.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>94</v>
       </c>

</xml_diff>